<commit_message>
modified height of rows in user acceptance test template
</commit_message>
<xml_diff>
--- a/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
+++ b/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\interlinkers-data\interlinkers\knowledge\User-Acceptance-Test-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9BCD1-59C8-4FE5-85E7-7BC6285F2BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092304F8-3542-4712-88D6-D326DE327444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,8 +1429,8 @@
   <dimension ref="A1:EY961"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68:B72"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="1:155" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:155" s="62" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="63"/>
       <c r="B15" s="66">
         <v>1</v>
@@ -1794,7 +1794,7 @@
       <c r="G15" s="49"/>
       <c r="H15" s="65"/>
     </row>
-    <row r="16" spans="1:155" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:155" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="63"/>
       <c r="B16" s="66">
         <v>2</v>
@@ -1810,7 +1810,7 @@
       <c r="G16" s="49"/>
       <c r="H16" s="65"/>
     </row>
-    <row r="17" spans="1:8" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="63"/>
       <c r="B17" s="66">
         <v>3</v>
@@ -1824,7 +1824,7 @@
       <c r="G17" s="49"/>
       <c r="H17" s="65"/>
     </row>
-    <row r="18" spans="1:8" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="62" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A18" s="63"/>
       <c r="B18" s="66">
         <v>4</v>
@@ -1840,7 +1840,7 @@
       <c r="G18" s="49"/>
       <c r="H18" s="65"/>
     </row>
-    <row r="19" spans="1:8" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="63"/>
       <c r="B19" s="66">
         <v>5</v>
@@ -1864,7 +1864,7 @@
       <c r="G20" s="31"/>
       <c r="H20" s="32"/>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="66">
         <v>1</v>
@@ -1882,7 +1882,7 @@
       <c r="G21" s="49"/>
       <c r="H21" s="28"/>
     </row>
-    <row r="22" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="69">
         <v>2</v>
@@ -1898,7 +1898,7 @@
       <c r="G22" s="50"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="69">
         <v>3</v>
@@ -1916,7 +1916,7 @@
       <c r="G23" s="50"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="69">
         <v>4</v>
@@ -1932,7 +1932,7 @@
       <c r="G24" s="50"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="69">
         <v>5</v>
@@ -1956,7 +1956,7 @@
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
     </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="66">
         <v>1</v>
@@ -1974,7 +1974,7 @@
       <c r="G27" s="49"/>
       <c r="H27" s="28"/>
     </row>
-    <row r="28" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="66">
         <f>B27+1</f>
@@ -1991,7 +1991,7 @@
       <c r="G28" s="50"/>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="66">
         <f t="shared" ref="B29:B49" si="0">B28+1</f>
@@ -2008,7 +2008,7 @@
       <c r="G29" s="50"/>
       <c r="H29" s="16"/>
     </row>
-    <row r="30" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="66">
         <f t="shared" si="0"/>
@@ -2025,7 +2025,7 @@
       <c r="G30" s="50"/>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="1:8" s="62" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="62" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A31" s="63"/>
       <c r="B31" s="66">
         <f t="shared" si="0"/>
@@ -2044,7 +2044,7 @@
       <c r="G31" s="50"/>
       <c r="H31" s="67"/>
     </row>
-    <row r="32" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="66">
         <f t="shared" si="0"/>
@@ -2061,7 +2061,7 @@
       <c r="G32" s="50"/>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="66">
         <f t="shared" si="0"/>
@@ -2078,7 +2078,7 @@
       <c r="G33" s="50"/>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="66">
         <f t="shared" si="0"/>
@@ -2095,7 +2095,7 @@
       <c r="G34" s="50"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="66">
         <f t="shared" si="0"/>
@@ -2112,7 +2112,7 @@
       <c r="G35" s="50"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="66">
         <f t="shared" si="0"/>
@@ -2129,7 +2129,7 @@
       <c r="G36" s="50"/>
       <c r="H36" s="16"/>
     </row>
-    <row r="37" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="66">
         <f t="shared" si="0"/>
@@ -2146,7 +2146,7 @@
       <c r="G37" s="50"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="66">
         <f t="shared" si="0"/>
@@ -2163,7 +2163,7 @@
       <c r="G38" s="50"/>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="66">
         <f t="shared" si="0"/>
@@ -2180,7 +2180,7 @@
       <c r="G39" s="50"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="66">
         <f t="shared" si="0"/>
@@ -2199,7 +2199,7 @@
       <c r="G40" s="50"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="66">
         <f>B40+1</f>
@@ -2216,7 +2216,7 @@
       <c r="G41" s="50"/>
       <c r="H41" s="16"/>
     </row>
-    <row r="42" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="66">
         <f t="shared" si="0"/>
@@ -2233,7 +2233,7 @@
       <c r="G42" s="50"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="66">
         <f t="shared" si="0"/>
@@ -2250,7 +2250,7 @@
       <c r="G43" s="50"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="66">
         <f t="shared" si="0"/>
@@ -2267,7 +2267,7 @@
       <c r="G44" s="50"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="66">
         <f t="shared" si="0"/>
@@ -2284,7 +2284,7 @@
       <c r="G45" s="50"/>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="66">
         <f t="shared" si="0"/>
@@ -2301,7 +2301,7 @@
       <c r="G46" s="50"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="66">
         <f t="shared" si="0"/>
@@ -2318,7 +2318,7 @@
       <c r="G47" s="50"/>
       <c r="H47" s="16"/>
     </row>
-    <row r="48" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="66">
         <f t="shared" si="0"/>
@@ -2337,7 +2337,7 @@
       <c r="G48" s="50"/>
       <c r="H48" s="16"/>
     </row>
-    <row r="49" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="66">
         <f t="shared" si="0"/>
@@ -2362,7 +2362,7 @@
       <c r="G50" s="31"/>
       <c r="H50" s="32"/>
     </row>
-    <row r="51" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="66">
         <v>1</v>
@@ -2380,7 +2380,7 @@
       <c r="G51" s="49"/>
       <c r="H51" s="28"/>
     </row>
-    <row r="52" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="69">
         <f>B51+1</f>
@@ -2397,7 +2397,7 @@
       <c r="G52" s="50"/>
       <c r="H52" s="16"/>
     </row>
-    <row r="53" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="69">
         <f t="shared" ref="B53:B57" si="1">B52+1</f>
@@ -2414,7 +2414,7 @@
       <c r="G53" s="50"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="69">
         <f t="shared" si="1"/>
@@ -2431,7 +2431,7 @@
       <c r="G54" s="50"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="69">
         <f t="shared" si="1"/>
@@ -2448,7 +2448,7 @@
       <c r="G55" s="50"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="69">
         <f t="shared" si="1"/>
@@ -2465,7 +2465,7 @@
       <c r="G56" s="50"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="69">
         <f t="shared" si="1"/>
@@ -2490,7 +2490,7 @@
       <c r="G58" s="31"/>
       <c r="H58" s="32"/>
     </row>
-    <row r="59" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="66">
         <v>1</v>
@@ -2508,7 +2508,7 @@
       <c r="G59" s="49"/>
       <c r="H59" s="28"/>
     </row>
-    <row r="60" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" s="8" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="66">
         <f>B59+1</f>
@@ -2525,7 +2525,7 @@
       <c r="G60" s="50"/>
       <c r="H60" s="16"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="66">
         <f t="shared" ref="B61:B66" si="2">B60+1</f>
@@ -2542,7 +2542,7 @@
       <c r="G61" s="50"/>
       <c r="H61" s="16"/>
     </row>
-    <row r="62" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="66">
         <f t="shared" si="2"/>
@@ -2559,7 +2559,7 @@
       <c r="G62" s="50"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="66">
         <f t="shared" si="2"/>
@@ -2576,7 +2576,7 @@
       <c r="G63" s="50"/>
       <c r="H63" s="16"/>
     </row>
-    <row r="64" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="66">
         <f t="shared" si="2"/>
@@ -2593,7 +2593,7 @@
       <c r="G64" s="50"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="66">
         <f t="shared" si="2"/>
@@ -2610,7 +2610,7 @@
       <c r="G65" s="50"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="66">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
added new task to verify that generated resources can be manipulated, e.g. cloned or deleted
</commit_message>
<xml_diff>
--- a/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
+++ b/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\interlinkers-data\interlinkers\knowledge\User-Acceptance-Test-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092304F8-3542-4712-88D6-D326DE327444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABDC28B-9E82-4856-A088-B34056581FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserAcceptance Testing TestCase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_ITEM4">'UserAcceptance Testing TestCase'!#REF!</definedName>
     <definedName name="_ITEM5">'UserAcceptance Testing TestCase'!#REF!</definedName>
     <definedName name="_ITEM6">'UserAcceptance Testing TestCase'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'UserAcceptance Testing TestCase'!$B$1:$H$80</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'UserAcceptance Testing TestCase'!$B$1:$H$81</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>Check recommended INTERLINKERs, e.g. go to ENGAGE&gt;Identify stakeholders&gt;Understand the different types of stakeholders. Ensure that the recommended INTELINKERS are viewable</t>
-  </si>
-  <si>
-    <t>You see a list of recommended INTERLINKERs, see what is behind each INTERLINKER by hovering the mouse over each INTERLINKER card. You should see a pop-up showing you a preview of the INTERLINKER</t>
   </si>
   <si>
     <t>Click on the INTERLINKER card, browse over its diverse tabs, click on button "Download locally as resource not related to project (for futures exploration)"</t>
@@ -416,6 +413,15 @@
   <si>
     <t>This template has been prepared by the INTERLINK European project,  is licensed under a Creative Commons Attribution-ShareAlike 4.0 International license (CC BY-SA 4.0). 
 This document remixes and builds upon the document provided by "Smartsheet" available at https://www.smartsheet.com/file/ic-user-acceptance-testing-test-case-template-10549xlsx.</t>
+  </si>
+  <si>
+    <t>You may Clone, Delete or Download a created resource by clicking on the pop-menu when clicking on 3 vertical dots under the Actions table header</t>
+  </si>
+  <si>
+    <t>Verify that a new resource appears when cloning, the existing one dissapears when deleting or that you download a copy of the resource when clicking on download</t>
+  </si>
+  <si>
+    <t>You see a list of recommended INTERLINKERs, see what is behind each INTERLINKER by hovering the mouse over each INTERLINKER card. You should see a pop-up showing you a preview of the INTERLINKER. Verify that the recommended INTERLINKERs are relevant.</t>
   </si>
 </sst>
 </file>
@@ -1087,9 +1093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2759075</xdr:colOff>
+      <xdr:colOff>2762250</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1426,11 +1432,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EY961"/>
+  <dimension ref="A1:EY962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1682,10 +1688,10 @@
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="62"/>
       <c r="F8" s="15"/>
@@ -1697,7 +1703,7 @@
       <c r="B9" s="15"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="54"/>
       <c r="F9" s="15"/>
@@ -1794,7 +1800,7 @@
       <c r="G15" s="49"/>
       <c r="H15" s="65"/>
     </row>
-    <row r="16" spans="1:155" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:155" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="63"/>
       <c r="B16" s="66">
         <v>2</v>
@@ -1855,7 +1861,7 @@
     <row r="20" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="30"/>
@@ -1882,7 +1888,7 @@
       <c r="G21" s="49"/>
       <c r="H21" s="28"/>
     </row>
-    <row r="22" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="69">
         <v>2</v>
@@ -1916,7 +1922,7 @@
       <c r="G23" s="50"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="69">
         <v>4</v>
@@ -1994,7 +2000,7 @@
     <row r="29" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="66">
-        <f t="shared" ref="B29:B49" si="0">B28+1</f>
+        <f t="shared" ref="B29:B50" si="0">B28+1</f>
         <v>3</v>
       </c>
       <c r="C29" s="64"/>
@@ -2019,7 +2025,7 @@
         <v>43</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="50"/>
@@ -2154,16 +2160,16 @@
       </c>
       <c r="C38" s="48"/>
       <c r="D38" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="59" t="s">
         <v>98</v>
-      </c>
-      <c r="E38" s="59" t="s">
-        <v>99</v>
       </c>
       <c r="F38" s="33"/>
       <c r="G38" s="50"/>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="8" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="66">
         <f t="shared" si="0"/>
@@ -2174,7 +2180,7 @@
         <v>60</v>
       </c>
       <c r="E39" s="59" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="50"/>
@@ -2187,13 +2193,13 @@
         <v>14</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="59" t="s">
         <v>62</v>
-      </c>
-      <c r="E40" s="59" t="s">
-        <v>63</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="50"/>
@@ -2207,10 +2213,10 @@
       </c>
       <c r="C41" s="48"/>
       <c r="D41" s="65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E41" s="59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="50"/>
@@ -2219,450 +2225,455 @@
     <row r="42" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B42:B50" si="1">B41+1</f>
         <v>16</v>
       </c>
       <c r="C42" s="48"/>
       <c r="D42" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="50"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C43" s="48"/>
       <c r="D43" s="65" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="E43" s="59" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="F43" s="33"/>
       <c r="G43" s="50"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C44" s="48"/>
       <c r="D44" s="65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E44" s="59" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F44" s="33"/>
       <c r="G44" s="50"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C45" s="48"/>
       <c r="D45" s="65" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E45" s="59" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="50"/>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C46" s="48"/>
       <c r="D46" s="65" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E46" s="59" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="50"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C47" s="48"/>
       <c r="D47" s="65" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E47" s="59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F47" s="33"/>
       <c r="G47" s="50"/>
       <c r="H47" s="16"/>
     </row>
-    <row r="48" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C48" s="64" t="s">
-        <v>82</v>
-      </c>
+      <c r="C48" s="48"/>
       <c r="D48" s="65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E48" s="59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="50"/>
       <c r="H48" s="16"/>
     </row>
-    <row r="49" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="65"/>
-      <c r="E49" s="59"/>
+      <c r="C49" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="59" t="s">
+        <v>80</v>
+      </c>
       <c r="F49" s="33"/>
       <c r="G49" s="50"/>
       <c r="H49" s="16"/>
     </row>
-    <row r="50" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="66">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C50" s="64"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="32"/>
+    </row>
+    <row r="52" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="66">
+        <v>1</v>
+      </c>
+      <c r="C52" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="32"/>
-    </row>
-    <row r="51" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="66">
-        <v>1</v>
-      </c>
-      <c r="C51" s="64" t="s">
+      <c r="D52" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="F51" s="34"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="28"/>
-    </row>
-    <row r="52" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="69">
-        <f>B51+1</f>
-        <v>2</v>
-      </c>
-      <c r="C52" s="48"/>
-      <c r="D52" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="E52" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="F52" s="33"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="F52" s="34"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="28"/>
+    </row>
+    <row r="53" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="69">
-        <f t="shared" ref="B53:B57" si="1">B52+1</f>
-        <v>3</v>
+        <f>B52+1</f>
+        <v>2</v>
       </c>
       <c r="C53" s="48"/>
       <c r="D53" s="65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E53" s="59" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F53" s="33"/>
       <c r="G53" s="50"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="69">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" ref="B54:B58" si="2">B53+1</f>
+        <v>3</v>
       </c>
       <c r="C54" s="48"/>
       <c r="D54" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="59" t="s">
         <v>90</v>
-      </c>
-      <c r="E54" s="59" t="s">
-        <v>92</v>
       </c>
       <c r="F54" s="33"/>
       <c r="G54" s="50"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="69">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="C55" s="48"/>
       <c r="D55" s="65" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E55" s="59" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F55" s="33"/>
       <c r="G55" s="50"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="69">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="C56" s="48"/>
       <c r="D56" s="65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E56" s="59" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F56" s="33"/>
       <c r="G56" s="50"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="69">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="C57" s="48"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="59"/>
+      <c r="D57" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" s="59" t="s">
+        <v>95</v>
+      </c>
       <c r="F57" s="33"/>
       <c r="G57" s="50"/>
       <c r="H57" s="16"/>
     </row>
-    <row r="58" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
-      <c r="B58" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="32"/>
-    </row>
-    <row r="59" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="B58" s="69">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C58" s="48"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
-      <c r="B59" s="66">
-        <v>1</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E59" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="F59" s="34"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="28"/>
-    </row>
-    <row r="60" spans="1:8" s="8" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="B59" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="32"/>
+    </row>
+    <row r="60" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="66">
-        <f>B59+1</f>
-        <v>2</v>
-      </c>
-      <c r="C60" s="48"/>
-      <c r="D60" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E60" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="F60" s="33"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="34"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="28"/>
+    </row>
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="66">
-        <f t="shared" ref="B61:B66" si="2">B60+1</f>
-        <v>3</v>
+        <f>B60+1</f>
+        <v>2</v>
       </c>
       <c r="C61" s="48"/>
       <c r="D61" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F61" s="33"/>
       <c r="G61" s="50"/>
       <c r="H61" s="16"/>
     </row>
-    <row r="62" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="66">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" ref="B62:B67" si="3">B61+1</f>
+        <v>3</v>
       </c>
       <c r="C62" s="48"/>
       <c r="D62" s="16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F62" s="33"/>
       <c r="G62" s="50"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="66">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="C63" s="48"/>
       <c r="D63" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E63" s="59" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F63" s="33"/>
       <c r="G63" s="50"/>
       <c r="H63" s="16"/>
     </row>
-    <row r="64" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="66">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="C64" s="48"/>
       <c r="D64" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E64" s="59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F64" s="33"/>
       <c r="G64" s="50"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="66">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
       <c r="C65" s="48"/>
       <c r="D65" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E65" s="59" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F65" s="33"/>
       <c r="G65" s="50"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="66">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="C66" s="48"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="59"/>
+      <c r="D66" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="59" t="s">
+        <v>114</v>
+      </c>
       <c r="F66" s="33"/>
       <c r="G66" s="50"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
-      <c r="B67" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="57"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="32"/>
+      <c r="B67" s="66">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C67" s="48"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="59"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="16"/>
     </row>
     <row r="68" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
-      <c r="B68" s="66">
-        <v>1</v>
-      </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="28"/>
+      <c r="B68" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="29"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="57"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="32"/>
     </row>
     <row r="69" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
-      <c r="B69" s="69">
-        <v>2</v>
-      </c>
-      <c r="C69" s="48"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="59"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="50"/>
-      <c r="H69" s="16"/>
+      <c r="B69" s="66">
+        <v>1</v>
+      </c>
+      <c r="C69" s="47"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="28"/>
     </row>
     <row r="70" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="48"/>
       <c r="D70" s="16"/>
@@ -2674,7 +2685,7 @@
     <row r="71" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" s="48"/>
       <c r="D71" s="16"/>
@@ -2686,7 +2697,7 @@
     <row r="72" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72" s="48"/>
       <c r="D72" s="16"/>
@@ -2695,41 +2706,43 @@
       <c r="G72" s="50"/>
       <c r="H72" s="16"/>
     </row>
-    <row r="73" spans="1:8" s="8" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="69">
+        <v>5</v>
+      </c>
+      <c r="C73" s="48"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="50"/>
+      <c r="H73" s="16"/>
+    </row>
+    <row r="74" spans="1:8" s="8" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C74" s="36"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="39"/>
-    </row>
-    <row r="75" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="41"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="42"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="60"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="39"/>
     </row>
     <row r="76" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
-      <c r="B76" s="44"/>
+      <c r="B76" s="43"/>
       <c r="C76" s="45"/>
       <c r="D76" s="40"/>
       <c r="E76" s="61"/>
@@ -2757,7 +2770,7 @@
       <c r="G78" s="41"/>
       <c r="H78" s="42"/>
     </row>
-    <row r="79" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="44"/>
       <c r="C79" s="45"/>
@@ -2777,17 +2790,17 @@
       <c r="G80" s="41"/>
       <c r="H80" s="42"/>
     </row>
-    <row r="81" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="61"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="42"/>
+    </row>
+    <row r="82" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -11586,6 +11599,16 @@
       <c r="F961" s="1"/>
       <c r="G961" s="1"/>
       <c r="H961" s="1"/>
+    </row>
+    <row r="962" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A962" s="1"/>
+      <c r="B962" s="1"/>
+      <c r="C962" s="1"/>
+      <c r="D962" s="1"/>
+      <c r="E962" s="55"/>
+      <c r="F962" s="1"/>
+      <c r="G962" s="1"/>
+      <c r="H962" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -11622,7 +11645,7 @@
     </row>
     <row r="5" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new testing tasks to User-Acceptance-Test-Template to acommodate it to new features introduced in collaborative environment
</commit_message>
<xml_diff>
--- a/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
+++ b/interlinkers/knowledge/User-Acceptance-Test-Template/resource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\interlinkers-data\interlinkers\knowledge\User-Acceptance-Test-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABDC28B-9E82-4856-A088-B34056581FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35AF11E-248B-40FB-8728-9CC75D57C1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserAcceptance Testing TestCase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_ITEM4">'UserAcceptance Testing TestCase'!#REF!</definedName>
     <definedName name="_ITEM5">'UserAcceptance Testing TestCase'!#REF!</definedName>
     <definedName name="_ITEM6">'UserAcceptance Testing TestCase'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'UserAcceptance Testing TestCase'!$B$1:$H$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'UserAcceptance Testing TestCase'!$B$1:$H$88</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="135">
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
@@ -108,9 +108,6 @@
     <t>Log into the Staging Server</t>
   </si>
   <si>
-    <t>Click on "Go to Dashboard" button</t>
-  </si>
-  <si>
     <t>Page Dashboard is rendered: https://demo.interlink-project.eu/dashboard</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Collaborative Environment shows the co-production process view, where users are requested to choose from the available co-production schemas</t>
   </si>
   <si>
-    <t>Browse through the proposed co.production tree schemas and choose one clicking on the corresponding "Use Schema" button</t>
-  </si>
-  <si>
     <t>The co-production process view of the dashboard now shows new menu items on the left-hand side, namely, Workplan &amp; Guide</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>USER ACCEPTANCE TESTING TEST CASE FOR COLLABORATIVE ENVIRONMENT</t>
   </si>
   <si>
-    <t>Observe the name, description, current status, recommended interlinkers (click on the arrow pointing downwards) and current set of resources created until that moment to complete such task</t>
-  </si>
-  <si>
     <t>Edit the selected task details by clicking on the PENCIL ICON</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>Check recommended INTERLINKERs, e.g. go to ENGAGE&gt;Identify stakeholders&gt;Understand the different types of stakeholders. Ensure that the recommended INTELINKERS are viewable</t>
   </si>
   <si>
-    <t>Click on the INTERLINKER card, browse over its diverse tabs, click on button "Download locally as resource not related to project (for futures exploration)"</t>
-  </si>
-  <si>
     <t xml:space="preserve">A version of the INTERLINKER in PDF, PPTX, DOCX … format so that you can see the enabler contents before using it </t>
   </si>
   <si>
@@ -363,12 +351,6 @@
     <t>Select one of the displayed INTERLINKERS by clicking on one an INTERLINKER card</t>
   </si>
   <si>
-    <t xml:space="preserve">A pop-up window should be shown. You may interact with the INTERLINKER by checking the tabs in case that the INTERLINKER is of software type: OVERVIEW, INSTRUCTIONS, REVIEWS and RELATED INTERLINKERS. The tabs available in the case of a KNOWLEDGE INTERLINKER are the same with the addition of the PREVIEW option which allows to download a desktop version of the resource. </t>
-  </si>
-  <si>
-    <t>Access to the permalink representing a given INTERLINKER by clickingo on the SHARE icon in a view of an INTERLINKER</t>
-  </si>
-  <si>
     <t>When pasting the URL copied in the clipboard into a browser you will get a full screen view of the INTERLINKER represented by that permalink</t>
   </si>
   <si>
@@ -376,9 +358,6 @@
   </si>
   <si>
     <t>Search for an INTERLINKER, e.g. type the keyword "Focus group"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 INTERLINKERs should be recommended an appear in the catalogue view of the Collaborative Environment </t>
   </si>
   <si>
     <t>Apply filters for nature which allows you to select among INTERLINKERS of the following categories INTERNAL SOFTWARE, INTERNAL KNOWLEDGE, EXTERNAL SOFTWARE and EXTERNAL KNOWLEDGE. Check 2 of  them.</t>
@@ -421,7 +400,64 @@
     <t>Verify that a new resource appears when cloning, the existing one dissapears when deleting or that you download a copy of the resource when clicking on download</t>
   </si>
   <si>
-    <t>You see a list of recommended INTERLINKERs, see what is behind each INTERLINKER by hovering the mouse over each INTERLINKER card. You should see a pop-up showing you a preview of the INTERLINKER. Verify that the recommended INTERLINKERs are relevant.</t>
+    <t>Browse through the proposed co.production tree schemas, preview them and choose one clicking on the corresponding "Use Schema" button</t>
+  </si>
+  <si>
+    <t>Observe the name, description, current status, recommended interlinkers (click on see recommended INTERLINKERs in the catalogue) and current set of resources created until that moment to complete such task</t>
+  </si>
+  <si>
+    <t>Log out by clicking on user icon at the top right hand side and then logout button</t>
+  </si>
+  <si>
+    <t>Pop up window appears asking you to confirm log out</t>
+  </si>
+  <si>
+    <t>Click on "Access to Dashboard" button</t>
+  </si>
+  <si>
+    <t>You see a list of recommended INTERLINKERs, see what is behind each INTERLINKER by clikcing on the title of each INTERLINKER card. You should see a pop-up showing you a preview of the INTERLINKER. Verify that the recommended INTERLINKERs are relevant.</t>
+  </si>
+  <si>
+    <t>Click on the INTERLINKER card, browse over its diverse tabs, click on button "Download locally as resource not related to project (for futures exploration)" or click on button "Download resource" of "Preview" tab</t>
+  </si>
+  <si>
+    <t>Create a fake co-production process, go to "Settings" left hand-side menu option, click on PENCIL icon and hit button "Remove coproduction process"</t>
+  </si>
+  <si>
+    <t>The co-producted process should be removed from the left hand-side of the dashboard view, You should not see the deleted project any longer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A pop-up window should be shown. You may interact with the INTERLINKER by checking the tabs in case that the INTERLINKER is of software type: OVERVIEW, INSTRUCTIONS, REVIEWS and RELATED INTERLINKERS. The tabs available in the case of an INTERNAL KNOWLEDGE INTERLINKER are the same with the addition of the PREVIEW option which allows to download a desktop version of the resource. </t>
+  </si>
+  <si>
+    <t>Access to the permalink representing a given INTERLINKER by clicking on the SHARE icon in a view of an INTERLINKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 4 INTERLINKERs should be recommended an appear in the catalogue view of the Collaborative Environment </t>
+  </si>
+  <si>
+    <t>Apply filter "Problem Profile", e.g. select ORG_PROBLEM_5</t>
+  </si>
+  <si>
+    <t>At least 2 INTERLINKERs meeting this problem profile should appear</t>
+  </si>
+  <si>
+    <t>Verify right documentation is shown</t>
+  </si>
+  <si>
+    <t>Click on "NEED HELP?" button on right hand side of screen. If not visible activate it in FILTERS icon top right hand side of screen and set ON "Show help button"</t>
+  </si>
+  <si>
+    <t>Ensure Dashboard documentation is shown</t>
+  </si>
+  <si>
+    <t>Ensure Co-production process documentation is shown. When you switch to OVERVIEW, GUIDE, WORKPLAN views, the corresponding HELP should be shown as pop up sliding window from right hand side of screen</t>
+  </si>
+  <si>
+    <t>Ensure Team management documentation is shown</t>
+  </si>
+  <si>
+    <t>Ensure Catalogue documentation is shown</t>
   </si>
 </sst>
 </file>
@@ -1432,11 +1468,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EY962"/>
+  <dimension ref="A1:EY969"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1490,7 @@
     <row r="1" spans="1:155" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1688,10 +1724,10 @@
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="13" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E8" s="62"/>
       <c r="F8" s="15"/>
@@ -1703,7 +1739,7 @@
       <c r="B9" s="15"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E9" s="54"/>
       <c r="F9" s="15"/>
@@ -1791,26 +1827,27 @@
         <v>17</v>
       </c>
       <c r="D15" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="58" t="s">
         <v>18</v>
-      </c>
-      <c r="E15" s="58" t="s">
-        <v>19</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="49"/>
       <c r="H15" s="65"/>
     </row>
-    <row r="16" spans="1:155" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:155" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="63"/>
       <c r="B16" s="66">
+        <f>B15+1</f>
         <v>2</v>
       </c>
       <c r="C16" s="64"/>
       <c r="D16" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="58" t="s">
         <v>20</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>21</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="49"/>
@@ -1819,11 +1856,12 @@
     <row r="17" spans="1:8" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="63"/>
       <c r="B17" s="66">
+        <f t="shared" ref="B17:B20" si="0">B16+1</f>
         <v>3</v>
       </c>
       <c r="C17" s="64"/>
       <c r="D17" s="65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="58"/>
       <c r="F17" s="33"/>
@@ -1833,303 +1871,311 @@
     <row r="18" spans="1:8" s="62" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A18" s="63"/>
       <c r="B18" s="66">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="58" t="s">
         <v>23</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>24</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="49"/>
       <c r="H18" s="65"/>
     </row>
-    <row r="19" spans="1:8" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="62" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="63"/>
       <c r="B19" s="66">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="58"/>
+      <c r="D19" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>118</v>
+      </c>
       <c r="F19" s="33"/>
       <c r="G19" s="49"/>
       <c r="H19" s="65"/>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="62" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="63"/>
+      <c r="B20" s="66">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="65"/>
+    </row>
+    <row r="21" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="66">
+      <c r="B21" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="66">
         <v>1</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C22" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="69">
-        <v>2</v>
-      </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="F22" s="34"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="69">
-        <v>3</v>
-      </c>
-      <c r="C23" s="64" t="s">
-        <v>30</v>
-      </c>
+        <f>B22+1</f>
+        <v>2</v>
+      </c>
+      <c r="C23" s="64"/>
       <c r="D23" s="65" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E23" s="59" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="50"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="69">
-        <v>4</v>
-      </c>
-      <c r="C24" s="64"/>
+        <f t="shared" ref="B24:B27" si="1">B23+1</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="64" t="s">
+        <v>29</v>
+      </c>
       <c r="D24" s="65" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="50"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="69">
-        <v>5</v>
-      </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="59"/>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>33</v>
+      </c>
       <c r="F25" s="33"/>
       <c r="G25" s="50"/>
       <c r="H25" s="16"/>
     </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
-    </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="69">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="33"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="66">
-        <v>1</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="28"/>
-    </row>
-    <row r="28" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="69">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C27" s="48"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="66">
-        <f>B27+1</f>
-        <v>2</v>
-      </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="66">
-        <f t="shared" ref="B29:B50" si="0">B28+1</f>
-        <v>3</v>
-      </c>
-      <c r="C29" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>35</v>
+      </c>
       <c r="D29" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="16"/>
+        <v>42</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="34"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="66">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>B29+1</f>
+        <v>2</v>
       </c>
       <c r="C30" s="64"/>
       <c r="D30" s="65" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="50"/>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="1:8" s="62" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="63"/>
+    <row r="31" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
       <c r="B31" s="66">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>42</v>
-      </c>
+        <f t="shared" ref="B31:B42" si="2">B30+1</f>
+        <v>3</v>
+      </c>
+      <c r="C31" s="64"/>
       <c r="D31" s="65" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E31" s="59" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="50"/>
-      <c r="H31" s="67"/>
-    </row>
-    <row r="32" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="66">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="C32" s="64"/>
       <c r="D32" s="65" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E32" s="59" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="50"/>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:8" s="62" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="63"/>
       <c r="B33" s="66">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C33" s="64"/>
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C33" s="64" t="s">
+        <v>40</v>
+      </c>
       <c r="D33" s="65" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E33" s="59" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="50"/>
-      <c r="H33" s="16"/>
+      <c r="H33" s="67"/>
     </row>
     <row r="34" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="66">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C34" s="48"/>
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="C34" s="64"/>
       <c r="D34" s="65" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E34" s="59" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="50"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="66">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C35" s="48"/>
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C35" s="64"/>
       <c r="D35" s="65" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E35" s="59" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="50"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="66">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="C36" s="48"/>
       <c r="D36" s="65" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E36" s="59" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F36" s="33"/>
       <c r="G36" s="50"/>
@@ -2138,411 +2184,421 @@
     <row r="37" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="66">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="C37" s="48"/>
       <c r="D37" s="65" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E37" s="59" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F37" s="33"/>
       <c r="G37" s="50"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="66">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="C38" s="48"/>
       <c r="D38" s="65" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="E38" s="59" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="F38" s="33"/>
       <c r="G38" s="50"/>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" s="8" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="66">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C39" s="48"/>
       <c r="D39" s="65" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E39" s="59" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="50"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="66">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>67</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="C40" s="48"/>
       <c r="D40" s="65" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="E40" s="59" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="50"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="8" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="66">
-        <f>B40+1</f>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="C41" s="48"/>
       <c r="D41" s="65" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E41" s="59" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="50"/>
       <c r="H41" s="16"/>
     </row>
-    <row r="42" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="66">
-        <f t="shared" ref="B42:B50" si="1">B41+1</f>
-        <v>16</v>
-      </c>
-      <c r="C42" s="48"/>
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>63</v>
+      </c>
       <c r="D42" s="65" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="50"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="66">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f>B42+1</f>
+        <v>15</v>
       </c>
       <c r="C43" s="48"/>
       <c r="D43" s="65" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E43" s="59" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="F43" s="33"/>
       <c r="G43" s="50"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="66">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f t="shared" ref="B44:B54" si="3">B43+1</f>
+        <v>16</v>
       </c>
       <c r="C44" s="48"/>
       <c r="D44" s="65" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E44" s="59" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F44" s="33"/>
       <c r="G44" s="50"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="66">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="3"/>
+        <v>17</v>
       </c>
       <c r="C45" s="48"/>
       <c r="D45" s="65" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="E45" s="59" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="50"/>
       <c r="H45" s="16"/>
     </row>
-    <row r="46" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="66">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
       <c r="C46" s="48"/>
       <c r="D46" s="65" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E46" s="59" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="50"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="8" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="66">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="C47" s="48"/>
       <c r="D47" s="65" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E47" s="59" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F47" s="33"/>
       <c r="G47" s="50"/>
       <c r="H47" s="16"/>
     </row>
-    <row r="48" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="66">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
       <c r="C48" s="48"/>
       <c r="D48" s="65" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E48" s="59" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="50"/>
       <c r="H48" s="16"/>
     </row>
-    <row r="49" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="66">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="C49" s="64" t="s">
-        <v>81</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="C49" s="48"/>
       <c r="D49" s="65" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F49" s="33"/>
       <c r="G49" s="50"/>
       <c r="H49" s="16"/>
     </row>
-    <row r="50" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="66">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="C50" s="64"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="59"/>
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="C50" s="48"/>
+      <c r="D50" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="59" t="s">
+        <v>74</v>
+      </c>
       <c r="F50" s="33"/>
       <c r="G50" s="50"/>
       <c r="H50" s="16"/>
     </row>
-    <row r="51" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
-      <c r="B51" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="32"/>
-    </row>
-    <row r="52" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="B51" s="66">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="C51" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="F51" s="33"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="66">
-        <v>1</v>
-      </c>
-      <c r="C52" s="64" t="s">
-        <v>83</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="C52" s="64"/>
       <c r="D52" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="E52" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="34"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="28"/>
-    </row>
-    <row r="53" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="E52" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="33"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
-      <c r="B53" s="69">
-        <f>B52+1</f>
-        <v>2</v>
-      </c>
-      <c r="C53" s="48"/>
+      <c r="B53" s="66">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="C53" s="64" t="s">
+        <v>129</v>
+      </c>
       <c r="D53" s="65" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="E53" s="59" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="F53" s="33"/>
       <c r="G53" s="50"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="69">
-        <f t="shared" ref="B54:B58" si="2">B53+1</f>
-        <v>3</v>
-      </c>
-      <c r="C54" s="48"/>
-      <c r="D54" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" s="59" t="s">
-        <v>90</v>
-      </c>
+      <c r="B54" s="66">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="C54" s="64"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="59"/>
       <c r="F54" s="33"/>
       <c r="G54" s="50"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
-      <c r="B55" s="69">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="F55" s="33"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="16"/>
-    </row>
-    <row r="56" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="32"/>
+    </row>
+    <row r="56" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
-      <c r="B56" s="69">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="C56" s="48"/>
+      <c r="B56" s="66">
+        <v>1</v>
+      </c>
+      <c r="C56" s="64" t="s">
+        <v>79</v>
+      </c>
       <c r="D56" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" s="33"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="16"/>
-    </row>
-    <row r="57" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="E56" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="34"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="28"/>
+    </row>
+    <row r="57" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="69">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>B56+1</f>
+        <v>2</v>
       </c>
       <c r="C57" s="48"/>
       <c r="D57" s="65" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E57" s="59" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F57" s="33"/>
       <c r="G57" s="50"/>
       <c r="H57" s="16"/>
     </row>
-    <row r="58" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="69">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f t="shared" ref="B58:B63" si="4">B57+1</f>
+        <v>3</v>
       </c>
       <c r="C58" s="48"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="59"/>
+      <c r="D58" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>86</v>
+      </c>
       <c r="F58" s="33"/>
       <c r="G58" s="50"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" s="8" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
-      <c r="B59" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="29"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="32"/>
-    </row>
-    <row r="60" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="B59" s="69">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="C59" s="48"/>
+      <c r="D59" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F59" s="33"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
-      <c r="B60" s="66">
-        <v>1</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="F60" s="34"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="28"/>
-    </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="B60" s="69">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="C60" s="48"/>
+      <c r="D60" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" s="33"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
-      <c r="B61" s="66">
-        <f>B60+1</f>
-        <v>2</v>
+      <c r="B61" s="69">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="C61" s="48"/>
-      <c r="D61" s="16" t="s">
-        <v>102</v>
+      <c r="D61" s="65" t="s">
+        <v>90</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F61" s="33"/>
       <c r="G61" s="50"/>
@@ -2550,327 +2606,372 @@
     </row>
     <row r="62" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
-      <c r="B62" s="66">
-        <f t="shared" ref="B62:B67" si="3">B61+1</f>
-        <v>3</v>
-      </c>
-      <c r="C62" s="48"/>
-      <c r="D62" s="16" t="s">
-        <v>104</v>
+      <c r="B62" s="69">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="C62" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="65" t="s">
+        <v>130</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="F62" s="33"/>
       <c r="G62" s="50"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
-      <c r="B63" s="66">
-        <f t="shared" si="3"/>
-        <v>4</v>
+      <c r="B63" s="69">
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="C63" s="48"/>
-      <c r="D63" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="59" t="s">
-        <v>108</v>
-      </c>
+      <c r="D63" s="65"/>
+      <c r="E63" s="59"/>
       <c r="F63" s="33"/>
       <c r="G63" s="50"/>
       <c r="H63" s="16"/>
     </row>
-    <row r="64" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
-      <c r="B64" s="66">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="C64" s="48"/>
-      <c r="D64" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E64" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="F64" s="33"/>
-      <c r="G64" s="50"/>
-      <c r="H64" s="16"/>
+      <c r="B64" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="29"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="32"/>
     </row>
     <row r="65" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="66">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="C65" s="48"/>
-      <c r="D65" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E65" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="F65" s="33"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E65" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="34"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="28"/>
+    </row>
+    <row r="66" spans="1:8" s="8" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="66">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <f>B65+1</f>
+        <v>2</v>
       </c>
       <c r="C66" s="48"/>
       <c r="D66" s="16" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E66" s="59" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F66" s="33"/>
       <c r="G66" s="50"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="66">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f t="shared" ref="B67:B74" si="5">B66+1</f>
+        <v>3</v>
       </c>
       <c r="C67" s="48"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="59"/>
+      <c r="D67" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>99</v>
+      </c>
       <c r="F67" s="33"/>
       <c r="G67" s="50"/>
       <c r="H67" s="16"/>
     </row>
-    <row r="68" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
-      <c r="B68" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C68" s="29"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="57"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="32"/>
-    </row>
-    <row r="69" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="66">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="C68" s="48"/>
+      <c r="D68" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E68" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F68" s="33"/>
+      <c r="G68" s="50"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="1:8" s="8" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="66">
-        <v>1</v>
-      </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="28"/>
-    </row>
-    <row r="70" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C69" s="48"/>
+      <c r="D69" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E69" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="F69" s="33"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" spans="1:8" s="8" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
-      <c r="B70" s="69">
-        <v>2</v>
+      <c r="B70" s="66">
+        <f t="shared" si="5"/>
+        <v>6</v>
       </c>
       <c r="C70" s="48"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="59"/>
+      <c r="D70" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" s="59" t="s">
+        <v>105</v>
+      </c>
       <c r="F70" s="33"/>
       <c r="G70" s="50"/>
       <c r="H70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
-      <c r="B71" s="69">
-        <v>3</v>
+      <c r="B71" s="66">
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="C71" s="48"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="59"/>
+      <c r="D71" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E71" s="59" t="s">
+        <v>128</v>
+      </c>
       <c r="F71" s="33"/>
       <c r="G71" s="50"/>
       <c r="H71" s="16"/>
     </row>
-    <row r="72" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" s="8" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
-      <c r="B72" s="69">
-        <v>4</v>
+      <c r="B72" s="66">
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="C72" s="48"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="59"/>
+      <c r="D72" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" s="59" t="s">
+        <v>107</v>
+      </c>
       <c r="F72" s="33"/>
       <c r="G72" s="50"/>
       <c r="H72" s="16"/>
     </row>
-    <row r="73" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" s="8" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
-      <c r="B73" s="69">
-        <v>5</v>
-      </c>
-      <c r="C73" s="48"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="59"/>
+      <c r="B73" s="66">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C73" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" s="59" t="s">
+        <v>134</v>
+      </c>
       <c r="F73" s="33"/>
       <c r="G73" s="50"/>
       <c r="H73" s="16"/>
     </row>
-    <row r="74" spans="1:8" s="8" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="35" t="s">
+    <row r="74" spans="1:8" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="66">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="C74" s="48"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="50"/>
+      <c r="H74" s="16"/>
+    </row>
+    <row r="75" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="57"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="32"/>
+    </row>
+    <row r="76" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="66">
+        <v>1</v>
+      </c>
+      <c r="C76" s="47"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="58"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="28"/>
+    </row>
+    <row r="77" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2"/>
+      <c r="B77" s="69">
+        <v>2</v>
+      </c>
+      <c r="C77" s="48"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="50"/>
+      <c r="H77" s="16"/>
+    </row>
+    <row r="78" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="69">
+        <v>3</v>
+      </c>
+      <c r="C78" s="48"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="50"/>
+      <c r="H78" s="16"/>
+    </row>
+    <row r="79" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="69">
+        <v>4</v>
+      </c>
+      <c r="C79" s="48"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="59"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="16"/>
+    </row>
+    <row r="80" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="69">
+        <v>5</v>
+      </c>
+      <c r="C80" s="48"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="16"/>
+    </row>
+    <row r="81" spans="1:8" s="8" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="36"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="60"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="39"/>
-    </row>
-    <row r="76" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="41"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="42"/>
-    </row>
-    <row r="77" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="61"/>
-      <c r="F77" s="41"/>
-      <c r="G77" s="41"/>
-      <c r="H77" s="42"/>
-    </row>
-    <row r="78" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="41"/>
-      <c r="G78" s="41"/>
-      <c r="H78" s="42"/>
-    </row>
-    <row r="79" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="44"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="40"/>
-      <c r="E79" s="61"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="41"/>
-      <c r="H79" s="42"/>
-    </row>
-    <row r="80" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="41"/>
-      <c r="G80" s="41"/>
-      <c r="H80" s="42"/>
-    </row>
-    <row r="81" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="44"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="41"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42"/>
-    </row>
-    <row r="82" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="55"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="55"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C82" s="36"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="60"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="39"/>
+    </row>
+    <row r="83" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="42"/>
+    </row>
+    <row r="84" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="45"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="61"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="41"/>
+      <c r="H84" s="42"/>
+    </row>
+    <row r="85" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="41"/>
+      <c r="G85" s="41"/>
+      <c r="H85" s="42"/>
+    </row>
+    <row r="86" spans="1:8" s="8" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="61"/>
+      <c r="F86" s="41"/>
+      <c r="G86" s="41"/>
+      <c r="H86" s="42"/>
+    </row>
+    <row r="87" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="61"/>
+      <c r="F87" s="41"/>
+      <c r="G87" s="41"/>
+      <c r="H87" s="42"/>
+    </row>
+    <row r="88" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="41"/>
+      <c r="G88" s="41"/>
+      <c r="H88" s="42"/>
+    </row>
+    <row r="89" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -11609,6 +11710,76 @@
       <c r="F962" s="1"/>
       <c r="G962" s="1"/>
       <c r="H962" s="1"/>
+    </row>
+    <row r="963" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A963" s="1"/>
+      <c r="B963" s="1"/>
+      <c r="C963" s="1"/>
+      <c r="D963" s="1"/>
+      <c r="E963" s="55"/>
+      <c r="F963" s="1"/>
+      <c r="G963" s="1"/>
+      <c r="H963" s="1"/>
+    </row>
+    <row r="964" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A964" s="1"/>
+      <c r="B964" s="1"/>
+      <c r="C964" s="1"/>
+      <c r="D964" s="1"/>
+      <c r="E964" s="55"/>
+      <c r="F964" s="1"/>
+      <c r="G964" s="1"/>
+      <c r="H964" s="1"/>
+    </row>
+    <row r="965" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A965" s="1"/>
+      <c r="B965" s="1"/>
+      <c r="C965" s="1"/>
+      <c r="D965" s="1"/>
+      <c r="E965" s="55"/>
+      <c r="F965" s="1"/>
+      <c r="G965" s="1"/>
+      <c r="H965" s="1"/>
+    </row>
+    <row r="966" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A966" s="1"/>
+      <c r="B966" s="1"/>
+      <c r="C966" s="1"/>
+      <c r="D966" s="1"/>
+      <c r="E966" s="55"/>
+      <c r="F966" s="1"/>
+      <c r="G966" s="1"/>
+      <c r="H966" s="1"/>
+    </row>
+    <row r="967" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A967" s="1"/>
+      <c r="B967" s="1"/>
+      <c r="C967" s="1"/>
+      <c r="D967" s="1"/>
+      <c r="E967" s="55"/>
+      <c r="F967" s="1"/>
+      <c r="G967" s="1"/>
+      <c r="H967" s="1"/>
+    </row>
+    <row r="968" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A968" s="1"/>
+      <c r="B968" s="1"/>
+      <c r="C968" s="1"/>
+      <c r="D968" s="1"/>
+      <c r="E968" s="55"/>
+      <c r="F968" s="1"/>
+      <c r="G968" s="1"/>
+      <c r="H968" s="1"/>
+    </row>
+    <row r="969" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A969" s="1"/>
+      <c r="B969" s="1"/>
+      <c r="C969" s="1"/>
+      <c r="D969" s="1"/>
+      <c r="E969" s="55"/>
+      <c r="F969" s="1"/>
+      <c r="G969" s="1"/>
+      <c r="H969" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -11645,7 +11816,7 @@
     </row>
     <row r="5" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="68" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>